<commit_message>
added size data and physical data and updated Rscript and output
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Seed_survivorship_and_sampling.xlsx
+++ b/RAnalysis/Data/Seed_survivorship_and_sampling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="12720" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="21540" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,8 +85,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -119,7 +123,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -133,6 +137,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -146,6 +152,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,7 +486,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -511,8 +519,7 @@
         <v>42445</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D6" ca="1" si="0">D8+2</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -526,8 +533,7 @@
         <v>42445</v>
       </c>
       <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -541,8 +547,7 @@
         <v>42445</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -556,8 +561,7 @@
         <v>42445</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -571,8 +575,7 @@
         <v>42445</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -586,8 +589,7 @@
         <v>42445</v>
       </c>
       <c r="D7">
-        <f>D13+2</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -601,7 +603,7 @@
         <v>42446</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D11" ca="1" si="1">D14+8</f>
+        <f t="shared" ref="D8:D12" si="0">D14+2</f>
         <v>45</v>
       </c>
       <c r="E8">
@@ -616,8 +618,8 @@
         <v>42446</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -631,7 +633,7 @@
         <v>42446</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="E10">
@@ -646,8 +648,8 @@
         <v>42446</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -661,8 +663,8 @@
         <v>42446</v>
       </c>
       <c r="D12">
-        <f ca="1">D18+8</f>
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -676,8 +678,8 @@
         <v>42446</v>
       </c>
       <c r="D13">
-        <f>D19+8</f>
-        <v>45</v>
+        <f>D19+2</f>
+        <v>48</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -691,8 +693,8 @@
         <v>42455</v>
       </c>
       <c r="D14">
-        <f ca="1">D8-E14</f>
-        <v>34</v>
+        <f t="shared" ref="D14:D18" si="1">D20+8</f>
+        <v>43</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -706,8 +708,8 @@
         <v>42455</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D18" ca="1" si="2">D9-E15</f>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="E15">
         <v>8</v>
@@ -721,7 +723,8 @@
         <v>42455</v>
       </c>
       <c r="D16">
-        <v>35</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="E16">
         <v>8</v>
@@ -735,8 +738,8 @@
         <v>42455</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="E17">
         <v>8</v>
@@ -750,8 +753,8 @@
         <v>42455</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>8</v>
@@ -765,7 +768,8 @@
         <v>42455</v>
       </c>
       <c r="D19">
-        <v>37</v>
+        <f>D25+8</f>
+        <v>46</v>
       </c>
       <c r="E19">
         <v>8</v>
@@ -778,6 +782,9 @@
       <c r="C20" s="1">
         <v>42468</v>
       </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
       <c r="E20">
         <v>0</v>
       </c>
@@ -789,6 +796,9 @@
       <c r="C21" s="1">
         <v>42468</v>
       </c>
+      <c r="D21">
+        <v>34</v>
+      </c>
       <c r="E21">
         <v>0</v>
       </c>
@@ -800,6 +810,9 @@
       <c r="C22" s="1">
         <v>42468</v>
       </c>
+      <c r="D22">
+        <v>33</v>
+      </c>
       <c r="E22">
         <v>0</v>
       </c>
@@ -811,6 +824,9 @@
       <c r="C23" s="1">
         <v>42468</v>
       </c>
+      <c r="D23">
+        <v>33</v>
+      </c>
       <c r="E23">
         <v>0</v>
       </c>
@@ -822,6 +838,9 @@
       <c r="C24" s="1">
         <v>42468</v>
       </c>
+      <c r="D24">
+        <v>32</v>
+      </c>
       <c r="E24">
         <v>0</v>
       </c>
@@ -832,6 +851,9 @@
       </c>
       <c r="C25" s="1">
         <v>42468</v>
+      </c>
+      <c r="D25">
+        <v>38</v>
       </c>
       <c r="E25">
         <v>0</v>

</xml_diff>